<commit_message>
Adjust find() function to locate non list items
</commit_message>
<xml_diff>
--- a/ECS.xlsx
+++ b/ECS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="9210" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="95">
   <si>
     <t>Sr#</t>
   </si>
@@ -149,36 +148,6 @@
     <t>http://10.67.82.22:4051/prov</t>
   </si>
   <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="AddSubscription"</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="ModifySubscriber"</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="DeleteSubscriber"</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:DeleteSubscriberRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-      &lt;/typ:DeleteSubscriberRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>DeleteSubscriberAPI</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="RemoveWallet"</t>
-  </si>
-  <si>
     <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
    &lt;soapenv:Header/&gt;
    &lt;soapenv:Body&gt;
@@ -306,9 +275,6 @@
   </si>
   <si>
     <t>GetECS</t>
-  </si>
-  <si>
-    <t>Clientsecret:i765cygre540i90uhyc5e64tyuiyfc</t>
   </si>
   <si>
     <t>{}</t>
@@ -352,10 +318,6 @@
 }</t>
   </si>
   <si>
-    <t>Clientsecret:i765cygre540i90uhyc5e64tyuiyfc
-Content-Type:application/json</t>
-  </si>
-  <si>
     <t>result_code_check_2001</t>
   </si>
   <si>
@@ -475,12 +437,43 @@
 ['ns3:test']['ns3:testlist'][1]['ns3:id']:2
 ['ns3:test']['ns3:testlist']:find(['ns3:id']:1;['ns3:name']:First)</t>
   </si>
+  <si>
+    <t>Content-Type=text/xml;charset=UTF-8;action="http://www.globe.com.ph/wsdl/SOAP/common/provisioning/v1/GetSubscriber"</t>
+  </si>
+  <si>
+    <t>GetECSSoap</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/ecssoap</t>
+  </si>
+  <si>
+    <t>['ns2:WalletList']=find(['Wallet']=PR_WNPGERALT_VRG;['State']=Active;['TotalAllocated'])
+['ns2:WalletList']=find(['Wallet']=PR_WNPGERALT_VRG;['State']=Terminated;['TotalAllocated'])</t>
+  </si>
+  <si>
+    <t>Content-Type=application/soap+xml;charset=UTF-8;action="AddSubscription"</t>
+  </si>
+  <si>
+    <t>Content-Type=application/soap+xml;charset=UTF-8;action="RemoveWallet"</t>
+  </si>
+  <si>
+    <t>Content-Type=application/soap+xml;charset=UTF-8;action="ModifyWalletState"</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>Clientsecret=765cygre540i90uhyc5e64tyuiyfc</t>
+  </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -623,6 +616,13 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -842,7 +842,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -968,14 +968,11 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1003,6 +1000,15 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="80">
@@ -1465,21 +1471,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="40.109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="21" customWidth="1"/>
     <col min="6" max="6" width="48" style="21" customWidth="1"/>
-    <col min="7" max="7" width="86.5546875" style="21" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="21"/>
+    <col min="7" max="7" width="86.5703125" style="21" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="25" customFormat="1" ht="45.75" customHeight="1">
@@ -1510,59 +1516,59 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.5">
       <c r="A3" s="21">
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="46.8">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="31.5">
       <c r="A4" s="21">
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>29</v>
+        <v>89</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75.75" customHeight="1">
@@ -1570,19 +1576,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>30</v>
+        <v>78</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>85</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75.75" customHeight="1">
@@ -1590,19 +1596,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>31</v>
+        <v>44</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>85</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="75.75" customHeight="1">
@@ -1610,7 +1616,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>4</v>
@@ -1619,10 +1625,10 @@
         <v>28</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>34</v>
+        <v>90</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="81" customHeight="1">
@@ -1630,7 +1636,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C8" s="23" t="s">
         <v>4</v>
@@ -1639,10 +1645,10 @@
         <v>28</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="57" customHeight="1">
@@ -1650,7 +1656,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>4</v>
@@ -1659,10 +1665,10 @@
         <v>28</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="57" customHeight="1">
@@ -1670,7 +1676,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>4</v>
@@ -1679,10 +1685,10 @@
         <v>28</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="G10" s="21" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="65.25" customHeight="1">
@@ -1690,7 +1696,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="23" t="s">
         <v>4</v>
@@ -1699,13 +1705,13 @@
         <v>28</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G11" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="405.6">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="409.5">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1730,10 +1736,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D13" s="27"/>
       <c r="F13" s="26"/>
@@ -1773,14 +1779,14 @@
     <hyperlink ref="D12" r:id="rId1"/>
     <hyperlink ref="D2" r:id="rId2"/>
     <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
-    <hyperlink ref="D3" r:id="rId10"/>
-    <hyperlink ref="D4" r:id="rId11"/>
+    <hyperlink ref="D7" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+    <hyperlink ref="D9" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D3" r:id="rId9"/>
+    <hyperlink ref="D4" r:id="rId10"/>
+    <hyperlink ref="D6" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
@@ -1789,35 +1795,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMO17"/>
+  <dimension ref="A1:AMO19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" style="6" customWidth="1"/>
     <col min="7" max="7" width="13" style="6" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="10" width="55.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="55.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" style="6" customWidth="1"/>
     <col min="13" max="14" width="21" style="6" customWidth="1"/>
-    <col min="15" max="1027" width="9.109375" style="12"/>
-    <col min="1028" max="1029" width="9.109375" style="13"/>
-    <col min="1030" max="16384" width="9.109375" style="7"/>
+    <col min="15" max="1027" width="9.140625" style="12"/>
+    <col min="1028" max="1029" width="9.140625" style="13"/>
+    <col min="1030" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1029" s="5" customFormat="1" ht="41.4">
+    <row r="1" spans="1:1029" s="5" customFormat="1" ht="38.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2876,28 +2882,28 @@
       <c r="AMN1" s="11"/>
       <c r="AMO1" s="11"/>
     </row>
-    <row r="2" spans="1:1029" ht="15.6">
+    <row r="2" spans="1:1029" ht="15.75">
       <c r="A2" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="48" t="s">
-        <v>62</v>
+      <c r="C2" s="47" t="s">
+        <v>54</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F2" s="31"/>
       <c r="G2" s="32"/>
       <c r="H2" s="33"/>
       <c r="I2" s="34"/>
       <c r="J2" s="34" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K2" s="32"/>
       <c r="L2" s="35"/>
@@ -2906,24 +2912,24 @@
     </row>
     <row r="3" spans="1:1029">
       <c r="A3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="49"/>
+        <v>42</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F3" s="31"/>
       <c r="G3" s="34"/>
       <c r="H3" s="34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I3" s="32"/>
       <c r="J3" s="34" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K3" s="32"/>
       <c r="L3" s="34"/>
@@ -2932,24 +2938,24 @@
     </row>
     <row r="4" spans="1:1029">
       <c r="A4" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49"/>
+        <v>56</v>
+      </c>
+      <c r="B4" s="57"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F4" s="31"/>
       <c r="G4" s="34"/>
       <c r="H4" s="34" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I4" s="32"/>
       <c r="J4" s="34" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K4" s="32"/>
       <c r="L4" s="34"/>
@@ -2958,24 +2964,24 @@
     </row>
     <row r="5" spans="1:1029">
       <c r="A5" s="28" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="49"/>
+        <v>57</v>
+      </c>
+      <c r="B5" s="57"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F5" s="31"/>
       <c r="G5" s="34"/>
       <c r="H5" s="34" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I5" s="32"/>
       <c r="J5" s="34" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="K5" s="32"/>
       <c r="L5" s="34"/>
@@ -2984,24 +2990,24 @@
     </row>
     <row r="6" spans="1:1029">
       <c r="A6" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="49"/>
+        <v>58</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="48"/>
       <c r="D6" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F6" s="31"/>
       <c r="G6" s="34"/>
       <c r="H6" s="34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I6" s="32"/>
       <c r="J6" s="34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K6" s="32"/>
       <c r="L6" s="34"/>
@@ -3010,52 +3016,54 @@
     </row>
     <row r="7" spans="1:1029">
       <c r="A7" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="50"/>
+        <v>59</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" s="49"/>
       <c r="D7" s="29" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="36" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F7" s="31"/>
       <c r="G7" s="34"/>
       <c r="H7" s="34" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I7" s="32"/>
       <c r="J7" s="34" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K7" s="32"/>
       <c r="L7" s="34"/>
       <c r="M7" s="34"/>
       <c r="N7" s="34"/>
     </row>
-    <row r="8" spans="1:1029" ht="15.6">
+    <row r="8" spans="1:1029" ht="15.75">
       <c r="A8" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="51">
+        <v>60</v>
+      </c>
+      <c r="B8" s="50">
         <v>2</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>74</v>
+      <c r="C8" s="53" t="s">
+        <v>66</v>
       </c>
       <c r="D8" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="38" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F8" s="39"/>
       <c r="G8" s="40"/>
       <c r="H8" s="41"/>
       <c r="I8" s="42"/>
       <c r="J8" s="42" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="K8" s="40"/>
       <c r="L8" s="43"/>
@@ -3064,24 +3072,24 @@
     </row>
     <row r="9" spans="1:1029">
       <c r="A9" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="55"/>
+        <v>61</v>
+      </c>
+      <c r="B9" s="51"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F9" s="39"/>
       <c r="G9" s="42"/>
       <c r="H9" s="42" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I9" s="40"/>
       <c r="J9" s="42" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K9" s="40"/>
       <c r="L9" s="42"/>
@@ -3090,24 +3098,24 @@
     </row>
     <row r="10" spans="1:1029">
       <c r="A10" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="55"/>
+        <v>68</v>
+      </c>
+      <c r="B10" s="51"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F10" s="39"/>
       <c r="G10" s="42"/>
       <c r="H10" s="42" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="I10" s="40"/>
       <c r="J10" s="42" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="K10" s="40"/>
       <c r="L10" s="42"/>
@@ -3116,52 +3124,52 @@
     </row>
     <row r="11" spans="1:1029">
       <c r="A11" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="55"/>
+        <v>69</v>
+      </c>
+      <c r="B11" s="51"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="44" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F11" s="39"/>
       <c r="G11" s="42"/>
       <c r="H11" s="42" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I11" s="40"/>
       <c r="J11" s="42" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="K11" s="40"/>
       <c r="L11" s="42"/>
       <c r="M11" s="42" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="N11" s="42"/>
     </row>
     <row r="12" spans="1:1029">
       <c r="A12" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="55"/>
+        <v>70</v>
+      </c>
+      <c r="B12" s="51"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F12" s="39"/>
       <c r="G12" s="42"/>
       <c r="H12" s="42" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I12" s="40"/>
       <c r="J12" s="42" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="K12" s="40"/>
       <c r="L12" s="42"/>
@@ -3170,116 +3178,161 @@
     </row>
     <row r="13" spans="1:1029">
       <c r="A13" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="56"/>
+        <v>71</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="55"/>
       <c r="D13" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="F13" s="39"/>
       <c r="G13" s="42"/>
       <c r="H13" s="42" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="I13" s="40"/>
       <c r="J13" s="42" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="K13" s="40"/>
       <c r="L13" s="42"/>
       <c r="M13" s="42"/>
       <c r="N13" s="42"/>
     </row>
-    <row r="14" spans="1:1029" ht="15.6">
+    <row r="14" spans="1:1029" ht="15.75">
       <c r="A14" s="28" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:1029" ht="15.6">
+    <row r="15" spans="1:1029" ht="15.75">
       <c r="A15" s="28" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B15" s="6">
         <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16"/>
       <c r="H15" s="18"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:1029" ht="15.6">
+    <row r="16" spans="1:1029" ht="15.75">
       <c r="A16" s="28" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B16" s="6">
         <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16"/>
       <c r="H16" s="18"/>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="1:11" ht="72">
+    <row r="17" spans="1:11" ht="75">
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>90</v>
+      <c r="B17" s="6">
+        <v>6</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D17" s="8">
         <v>200</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="60">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="8">
+        <v>200</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="J18" s="46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="6">
+        <v>17</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="8">
+        <v>200</v>
+      </c>
+      <c r="E19" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="31"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="32"/>
+      <c r="J19" s="34" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B7"/>
+  <mergeCells count="3">
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="C8:C13"/>

</xml_diff>

<commit_message>
Add Changes for compool
</commit_message>
<xml_diff>
--- a/ECS.xlsx
+++ b/ECS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
   <si>
     <t>Sr#</t>
   </si>
@@ -110,195 +109,9 @@
     <t>Post_Commands</t>
   </si>
   <si>
-    <t>RegularRecharge</t>
-  </si>
-  <si>
-    <t>http://10.225.10.9:8011/replenishment</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="RegularRecharge"</t>
-  </si>
-  <si>
-    <t>&lt;soap:Envelope xmlns:soap="http://www.w3.org/2003/05/soap-envelope" xmlns:rep="http://www.globe.com/warcraft/wsdl/replenishment/"&gt;
-   &lt;soap:Header/&gt;
-   &lt;soap:Body&gt;
-      &lt;rep:RegularRecharge&gt;
-         &lt;BaseChannel&gt;
-            &lt;ReferenceId&gt;RPL9_AMAX&lt;/ReferenceId&gt;
-            &lt;RequestDateTime&gt;2020-01-30T00:00:00&lt;/RequestDateTime&gt;
-            &lt;TransactionId&gt;12345&lt;/TransactionId&gt;
-         &lt;/BaseChannel&gt;
-         &lt;BaseRegularRecharge&gt;
-            &lt;Amount&gt;10&lt;/Amount&gt;
-            &lt;Currency&gt;PHP&lt;/Currency&gt;
-         &lt;/BaseRegularRecharge&gt;
-         &lt;Subscriber&gt;
-            &lt;PrimaryResourceType&gt;c&lt;/PrimaryResourceType&gt;
-            &lt;PrimaryResourceValue&gt;9270910049&lt;/PrimaryResourceValue&gt;
-         &lt;/Subscriber&gt;
-         &lt;Method&gt;
-            &lt;MethodName&gt;NA&lt;/MethodName&gt;
-            &lt;ReasonCode&gt;NA&lt;/ReasonCode&gt;
-         &lt;/Method&gt;
-         &lt;SendSMS&gt;false&lt;/SendSMS&gt;
-      &lt;/rep:RegularRecharge&gt;
-   &lt;/soap:Body&gt;
-&lt;/soap:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>http://10.67.82.22:4051/prov</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="AddSubscription"</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="ModifySubscriber"</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="DeleteSubscriber"</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:DeleteSubscriberRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-      &lt;/typ:DeleteSubscriberRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>DeleteSubscriberAPI</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="RemoveWallet"</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:RemoveWalletRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-         &lt;typ:Wallet&gt;#{wallet}#&lt;/typ:Wallet&gt;
-      &lt;/typ:RemoveWalletRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>RemoveWalletAPI</t>
-  </si>
-  <si>
-    <t>ModifyWalletStateAPI</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="ModifyWalletState"</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:ModifyWalletStateRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-         &lt;typ:Wallet&gt;#{wallet}#&lt;/typ:Wallet&gt;
-         &lt;typ:State&gt;#{state}#&lt;/typ:State&gt;
-      &lt;/typ:ModifyWalletStateRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>ExtendValiditityOfWalletAPI</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:ExtendValidityOfWalletRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-         &lt;typ:Wallet&gt;#{wallet}#&lt;/typ:Wallet&gt;
-         &lt;typ:ValidityUnit&gt;Days&lt;/typ:ValidityUnit&gt;
-         &lt;typ:ValidityValue&gt;#{days}#&lt;/typ:ValidityValue&gt;
-      &lt;/typ:ExtendValidityOfWalletRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:IncrementWalletRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-         &lt;typ:Wallet&gt;#{wallet}#&lt;/typ:Wallet&gt;
-         &lt;typ:Amount&gt;#{increment}#&lt;/typ:Amount&gt;
-         &lt;typ:Unit&gt;KB&lt;/typ:Unit&gt;
-         &lt;typ:IsRollback&gt;0&lt;/typ:IsRollback&gt;
-         &lt;typ:Duration&gt;60&lt;/typ:Duration&gt;
-      &lt;/typ:IncrementWalletRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
-    <t>IncrementWalletAPI</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="IncrementWallet"</t>
-  </si>
-  <si>
-    <t>DecrementWalletAPI</t>
-  </si>
-  <si>
-    <t>Content-Type: application/soap+xml;charset=UTF-8;action="DecrementWallet"</t>
-  </si>
-  <si>
-    <t>&lt;soapenv:Envelope xmlns:soapenv="http://schemas.xmlsoap.org/soap/envelope/" xmlns:typ="http://www.globe.com.ph/schemas/SOAP/provisioning/subscriber/v1/types" xmlns:typ1="http://www.globe.com.ph/schemas/SOAP/provisioning/common/v1/types"&gt;
-   &lt;soapenv:Header/&gt;
-   &lt;soapenv:Body&gt;
-      &lt;typ:DecrementWalletRequest&gt;
-         &lt;typ:Header&gt;
-            &lt;typ1:Timestamp&gt;2022-01-03T11:59:00&lt;/typ1:Timestamp&gt;
-            &lt;typ1:Source&gt;Tech Team Script&lt;/typ1:Source&gt;
-            &lt;typ1:TransactionId&gt;script_2022-01-03T11:59:00&lt;/typ1:TransactionId&gt;
-         &lt;/typ:Header&gt;
-         &lt;typ:MSISDN&gt;#{msisdn}#&lt;/typ:MSISDN&gt;
-         &lt;typ:Wallet&gt;#{wallet}#&lt;/typ:Wallet&gt;
-         &lt;typ:Amount&gt;#{decrement}#&lt;/typ:Amount&gt;
-         &lt;typ:Unit&gt;KB&lt;/typ:Unit&gt;
-         &lt;typ:IsRollback&gt;0&lt;/typ:IsRollback&gt;
-      &lt;/typ:DecrementWalletRequest&gt;
-   &lt;/soapenv:Body&gt;
-&lt;/soapenv:Envelope&gt;</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
-    <t>GetSubscriberAPI2</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -306,9 +119,6 @@
   </si>
   <si>
     <t>GetECS</t>
-  </si>
-  <si>
-    <t>Clientsecret:i765cygre540i90uhyc5e64tyuiyfc</t>
   </si>
   <si>
     <t>{}</t>
@@ -352,10 +162,6 @@
 }</t>
   </si>
   <si>
-    <t>Clientsecret:i765cygre540i90uhyc5e64tyuiyfc
-Content-Type:application/json</t>
-  </si>
-  <si>
     <t>result_code_check_2001</t>
   </si>
   <si>
@@ -371,9 +177,6 @@
     <t>Test Case #1: 5 API Calls</t>
   </si>
   <si>
-    <t>session_id:Step1</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -392,22 +195,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>session_id:Step2</t>
-  </si>
-  <si>
-    <t>session_id:Step3</t>
-  </si>
-  <si>
-    <t>session_id:Step4</t>
-  </si>
-  <si>
-    <t>session_id:Step5</t>
-  </si>
-  <si>
     <t>Test Case #1: 5 API Calls (Last 2 Skipped)</t>
-  </si>
-  <si>
-    <t>session_id:Invalid</t>
   </si>
   <si>
     <t>9</t>
@@ -463,24 +251,335 @@
 &lt;/soapenv:Envelope&gt;</t>
   </si>
   <si>
+    <t>http://127.0.0.1:5000/ecssoap</t>
+  </si>
+  <si>
+    <t>GetECSSoap</t>
+  </si>
+  <si>
+    <t>Content-Type=application/soap+xml;charset=UTF-8;action="ModifySubscriber"</t>
+  </si>
+  <si>
+    <t>Content-Type=application/soap+xml;charset=UTF-8;action="AddSubscription"</t>
+  </si>
+  <si>
+    <t>Clientsecret=i765cygre540i90uhyc5e64tyuiyfc
+Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>Clientsecret=i765cygre540i90uhyc5e64tyuiyfc</t>
+  </si>
+  <si>
+    <t>session_id=Step1</t>
+  </si>
+  <si>
+    <t>session_id=Step2</t>
+  </si>
+  <si>
+    <t>session_id=Step3</t>
+  </si>
+  <si>
+    <t>session_id=Step4</t>
+  </si>
+  <si>
+    <t>session_id=Step5</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>session_id=Invalid</t>
+  </si>
+  <si>
+    <t>['ns3:EndDate']=addTime(#{StartDate}#, 3days)</t>
+  </si>
+  <si>
+    <t>StartDate=['ns3:StartDate']</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>initData</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/init</t>
+  </si>
+  <si>
+    <t>Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>updateData</t>
+  </si>
+  <si>
+    <t>terminateData</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/update</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:5000/terminate</t>
+  </si>
+  <si>
+    <t>Failing Report</t>
+  </si>
+  <si>
+    <t>Passing Report</t>
+  </si>
+  <si>
+    <t>webvalidation_NFPromo_9270990234_Active_7_API_Passing</t>
+  </si>
+  <si>
     <t>1(Start)(End)</t>
   </si>
   <si>
-    <t>startDate:['ns3:StartDate']</t>
-  </si>
-  <si>
-    <t>['ns3:EndDate']:addTime(#{startDate}#,3days)
-['ns3:test']['ns3:testlist'][0]['ns3:id']:1
-['ns3:test']['ns3:testlist'][0]['ns3:name']:First
-['ns3:test']['ns3:testlist'][1]['ns3:id']:2
-['ns3:test']['ns3:testlist']:find(['ns3:id']:1;['ns3:name']:First)</t>
+    <t>consume_data_2699.1mb</t>
+  </si>
+  <si>
+    <t>['ns3:MemberList']=find(['MSISDN']=639270990232;['TotalAllocated'];storeIndexTo=memberIndex)
+allocatedValue=get_value(['ns3:MemberList'];['TotalAllocated'];memberIndex)</t>
+  </si>
+  <si>
+    <t>test_case_prefix=Send Group status</t>
+  </si>
+  <si>
+    <t>test_case_postfix=for consumption</t>
+  </si>
+  <si>
+    <t>test_case_prefix=Send Member status
+test_case_postfix=for group 1</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>{
+    "session_id": "tb_ugwgy01;3759037027;380;16784224",
+    "origin_host": "TB_UGWGY03",
+    "origin_realm": "ugw.gy.globe.ph",
+    "destination_realm": "sigm.gy.globe.com.ph",
+    "auth_application_id": "4",
+    "service_context_id": "32270@3gpp.org",
+    "cc_request_type": "1",
+    "cc_request_number": "1",
+    "destination_host": "vmsnmadv01-rtsm",
+    "user_name": "0",
+    "origin_state_id": "3725150938",
+    "event_timestamp": "1549893870",
+    "filler": "0",
+    "subscription_id_type": "0",
+    "subscription_id_data": "639270990234",
+    "multiple_services_indicator": "1",
+    "filler": "0",
+    "service_identifier": "3",
+    "rating_group": "650",
+    "cc_time": "10",
+    "cc_total_octets": "0",
+    "cc_input_octets": "5120",
+    "cc_output_octets": "5120",
+    "filler": "0",
+    "filler": "0",
+    "reporting_reason": "3",
+    "requested_service_unit": "0",
+    "user_equipment_info_type": "0",
+    "user_equipment_info_value": "3562020959759701",
+    "pdp_address": "10.178.145.131",
+    "called_station_id": "tbturismo.internet.globe.com.ph",
+    "3gpp_imsi_mcc_mnc": "51502",
+    "ggsn_address": "112.198.110.25",
+    "sgsn_address": "10.178.130.241",
+    "3gpp_charging_id": "662701960",
+    "3gpp_gprs_negotiated_qos_profile": "08-2d06000186a0000493e0",
+    "3gpp_charging_characteristic": "0800",
+    "3gpp_pdp_type": "0",
+    "3gpp_sgsn_mcc_mnc": "51502",
+    "3gpp_imsi_mcc_mnc": "51502",
+    "cg_address": "10.178.130.241",
+    "3gpp_ggsn_mcc_mnc": "51502",
+    "3gpp_nsapi": "5",
+    "3gpp_selection_mode": "0",
+    "3gpp_rat_type": "06",
+    "3gpp_user_location_info": "8215f520001815f52001b8db0c",
+    "pdp_context_type": "0",
+    "host": "127.0.0.1",
+    "port": 5007
+}</t>
+  </si>
+  <si>
+    <t>{
+    "session_id": "tb_ugwgy01;3759037027;380;16784224",
+    "origin_host": "TB_UGWGY03",
+    "origin_realm": "ugw.gy.globe.ph",
+    "destination_realm": "sigm.gy.globe.com.ph",
+    "auth_application_id": "4",
+    "service_context_id": "32270@3gpp.org",
+    "cc_request_type": "3",
+    "cc_request_number": "1",
+    "destination_host": "vmsnmadv01-rtsm",
+    "user_name": "0",
+    "origin_state_id": "3725150938",
+    "event_timestamp": "1549893870",
+    "filler": "0",
+    "subscription_id_type": "0",
+    "subscription_id_data": "639270990234",
+    "multiple_services_indicator": "1",
+    "filler": "0",
+    "service_identifier": "3",
+    "rating_group": "650",
+    "cc_time": "10",
+    "cc_total_octets": "0",
+    "cc_input_octets": "5120",
+    "cc_output_octets": "5120",
+    "filler": "0",
+    "filler": "0",
+    "reporting_reason": "3",
+    "requested_service_unit": "0",
+    "user_equipment_info_type": "0",
+    "user_equipment_info_value": "3562020959759701",
+    "pdp_address": "10.178.145.131",
+    "called_station_id": "tbturismo.internet.globe.com.ph",
+    "3gpp_imsi_mcc_mnc": "51502",
+    "ggsn_address": "112.198.110.25",
+    "sgsn_address": "10.178.130.241",
+    "3gpp_charging_id": "662701960",
+    "3gpp_gprs_negotiated_qos_profile": "08-2d06000186a0000493e0",
+    "3gpp_charging_characteristic": "0800",
+    "3gpp_pdp_type": "0",
+    "3gpp_sgsn_mcc_mnc": "51502",
+    "3gpp_imsi_mcc_mnc": "51502",
+    "cg_address": "10.178.130.241",
+    "3gpp_ggsn_mcc_mnc": "51502",
+    "3gpp_nsapi": "5",
+    "3gpp_selection_mode": "0",
+    "3gpp_rat_type": "06",
+    "3gpp_user_location_info": "8215f520001815f52001b8db0c",
+    "pdp_context_type": "0",
+    "host": "127.0.0.1",
+    "port": 5007
+}</t>
+  </si>
+  <si>
+    <t>{
+    "session_id": "tb_ugwgy01;3759037027;380;16784224",
+    "origin_host": "TB_UGWGY03",
+    "origin_realm": "ugw.gy.globe.ph",
+    "destination_realm": "sigm.gy.globe.com.ph",
+    "auth_application_id": "4",
+    "service_context_id": "32270@3gpp.org",
+    "cc_request_type": "2",
+    "cc_request_number": "1",
+    "destination_host": "vmsnmadv01-rtsm",
+    "user_name": "0",
+    "origin_state_id": "3725150938",
+    "event_timestamp": "1549893870",
+    "filler": "0",
+    "subscription_id_type": "0",
+    "subscription_id_data": "639270990234",
+    "multiple_services_indicator": "1",
+    "filler": "0",
+    "service_identifier": "3",
+    "rating_group": "650",
+    "cc_time": "10",
+    "cc_total_octets": "0",
+    "cc_input_octets": "5120",
+    "cc_output_octets": "5120",
+    "filler": "0",
+    "filler": "0",
+    "reporting_reason": "3",
+    "requested_service_unit": "0",
+    "user_equipment_info_type": "0",
+    "user_equipment_info_value": "3562020959759701",
+    "pdp_address": "10.178.145.131",
+    "called_station_id": "tbturismo.internet.globe.com.ph",
+    "3gpp_imsi_mcc_mnc": "51502",
+    "ggsn_address": "112.198.110.25",
+    "sgsn_address": "10.178.130.241",
+    "3gpp_charging_id": "662701960",
+    "3gpp_gprs_negotiated_qos_profile": "08-2d06000186a0000493e0",
+    "3gpp_charging_characteristic": "0800",
+    "3gpp_pdp_type": "0",
+    "3gpp_sgsn_mcc_mnc": "51502",
+    "3gpp_imsi_mcc_mnc": "51502",
+    "cg_address": "10.178.130.241",
+    "3gpp_ggsn_mcc_mnc": "51502",
+    "3gpp_nsapi": "5",
+    "3gpp_selection_mode": "0",
+    "3gpp_rat_type": "06",
+    "3gpp_user_location_info": "8215f520001815f52001b8db0c",
+    "pdp_context_type": "0",
+    "host": "127.0.0.1",
+    "port": 5007
+}</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>ConsumeDataFailing</t>
+  </si>
+  <si>
+    <t>ConsumeDataPassing</t>
+  </si>
+  <si>
+    <t>webvalidation_NFPromo_9270990234_Active_7_API_Failing</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>API Passing with Prefix</t>
+  </si>
+  <si>
+    <t>API Passing with Prefix and Postfix</t>
+  </si>
+  <si>
+    <t>API Passing with Postfix</t>
+  </si>
+  <si>
+    <t>API Failing Status Code</t>
+  </si>
+  <si>
+    <t>API Failing Validation</t>
+  </si>
+  <si>
+    <t>API Passing without Prefix or Postfix</t>
+  </si>
+  <si>
+    <t>session_id=Step7</t>
+  </si>
+  <si>
+    <t>10(End)</t>
+  </si>
+  <si>
+    <t>['ns3:MemberList']=find(['MSISDN']=639270s990232;['TotalAllocated'])</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -617,11 +716,6 @@
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -842,7 +936,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -915,9 +1009,6 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="79" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -969,13 +1060,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1002,6 +1096,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1463,23 +1560,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" style="21" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="40.109375" style="21" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="21" customWidth="1"/>
     <col min="6" max="6" width="48" style="21" customWidth="1"/>
-    <col min="7" max="7" width="86.5546875" style="21" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="21"/>
+    <col min="7" max="7" width="86.5703125" style="21" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="25" customFormat="1" ht="45.75" customHeight="1">
@@ -1510,59 +1607,59 @@
         <v>1</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.5">
       <c r="A3" s="21">
         <v>2</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>51</v>
+      <c r="D3" s="26" t="s">
+        <v>26</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="46.8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="47.25">
       <c r="A4" s="21">
         <v>3</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>29</v>
-      </c>
       <c r="G4" s="21" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="75.75" customHeight="1">
@@ -1570,19 +1667,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>86</v>
+        <v>25</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>53</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="75.75" customHeight="1">
@@ -1590,234 +1687,146 @@
         <v>5</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>57</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="75.75" customHeight="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="409.5">
       <c r="A7" s="21">
         <v>6</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>36</v>
+      <c r="B7" s="22" t="s">
+        <v>73</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>74</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="81" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="409.5">
       <c r="A8" s="21">
         <v>7</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>37</v>
+      <c r="B8" s="22" t="s">
+        <v>76</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>78</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="409.5">
       <c r="A9" s="21">
         <v>8</v>
       </c>
-      <c r="B9" s="21" t="s">
-        <v>40</v>
+      <c r="B9" s="22" t="s">
+        <v>77</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="26" t="s">
+        <v>79</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="57" customHeight="1">
-      <c r="A10" s="21">
-        <v>9</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="65.25" customHeight="1">
-      <c r="A11" s="21">
-        <v>10</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="405.6">
-      <c r="A12" s="21">
-        <v>11</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>27</v>
-      </c>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10" s="23"/>
+      <c r="D10" s="24"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" s="23"/>
+      <c r="D11" s="24"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="21">
-        <v>12</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="F13" s="26"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="C14" s="23"/>
       <c r="D14" s="24"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="C15" s="23"/>
-      <c r="D15" s="24"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" s="23"/>
-      <c r="D16" s="24"/>
-    </row>
-    <row r="17" spans="3:4">
-      <c r="C17" s="23"/>
-      <c r="D17" s="24"/>
-    </row>
-    <row r="18" spans="3:4">
-      <c r="C18" s="23"/>
-      <c r="D18" s="24"/>
-    </row>
-    <row r="19" spans="3:4">
-      <c r="D19" s="24"/>
-    </row>
-    <row r="20" spans="3:4">
-      <c r="D20" s="24"/>
-    </row>
-    <row r="21" spans="3:4">
-      <c r="D21" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="D9" r:id="rId7"/>
-    <hyperlink ref="D10" r:id="rId8"/>
-    <hyperlink ref="D11" r:id="rId9"/>
-    <hyperlink ref="D3" r:id="rId10"/>
-    <hyperlink ref="D4" r:id="rId11"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMO17"/>
+  <dimension ref="A1:AMO28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.88671875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="36" style="6" customWidth="1"/>
     <col min="7" max="7" width="13" style="6" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" style="6" customWidth="1"/>
     <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="10" width="55.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="23.21875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="55.7109375" style="6" customWidth="1"/>
+    <col min="11" max="11" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="21" style="6" customWidth="1"/>
-    <col min="15" max="1027" width="9.109375" style="12"/>
-    <col min="1028" max="1029" width="9.109375" style="13"/>
-    <col min="1030" max="16384" width="9.109375" style="7"/>
+    <col min="15" max="1027" width="9.140625" style="12"/>
+    <col min="1028" max="1029" width="9.140625" style="13"/>
+    <col min="1030" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1029" s="5" customFormat="1" ht="41.4">
+    <row r="1" spans="1:1029" s="5" customFormat="1" ht="38.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -2876,410 +2885,711 @@
       <c r="AMN1" s="11"/>
       <c r="AMO1" s="11"/>
     </row>
-    <row r="2" spans="1:1029" ht="15.6">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:1029" ht="15.75">
+      <c r="A2" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="44" t="s">
         <v>21</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="35"/>
-    </row>
-    <row r="3" spans="1:1029">
-      <c r="A3" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="46"/>
+      <c r="E2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="31"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="31"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="34"/>
+    </row>
+    <row r="3" spans="1:1029" ht="30">
+      <c r="A3" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>68</v>
+      </c>
       <c r="C3" s="49"/>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="31"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34" t="s">
+      <c r="E3" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="34" t="s">
+      <c r="I3" s="31"/>
+      <c r="J3" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
     </row>
     <row r="4" spans="1:1029">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="29" t="s">
+      <c r="I4" s="31"/>
+      <c r="J4" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="31"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+    </row>
+    <row r="5" spans="1:1029">
+      <c r="A5" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="31"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="32"/>
-      <c r="J4" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-    </row>
-    <row r="5" spans="1:1029">
-      <c r="A5" s="28" t="s">
+      <c r="E5" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="29" t="s">
+      <c r="I5" s="31"/>
+      <c r="J5" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="31"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+    </row>
+    <row r="6" spans="1:1029">
+      <c r="A6" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="45"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="31"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-    </row>
-    <row r="6" spans="1:1029">
-      <c r="A6" s="28" t="s">
+      <c r="E6" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="30"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="46"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="29" t="s">
+      <c r="I6" s="31"/>
+      <c r="J6" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K6" s="31"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+      <c r="N6" s="33"/>
+    </row>
+    <row r="7" spans="1:1029">
+      <c r="A7" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="46"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="31"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="I6" s="32"/>
-      <c r="J6" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="34"/>
-      <c r="M6" s="34"/>
-      <c r="N6" s="34"/>
-    </row>
-    <row r="7" spans="1:1029">
-      <c r="A7" s="28" t="s">
+      <c r="E7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-    </row>
-    <row r="8" spans="1:1029" ht="15.6">
-      <c r="A8" s="28" t="s">
-        <v>68</v>
+      <c r="I7" s="31"/>
+      <c r="J7" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="31"/>
+      <c r="L7" s="33"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="33"/>
+    </row>
+    <row r="8" spans="1:1029" ht="15.75">
+      <c r="A8" s="27" t="s">
+        <v>40</v>
       </c>
       <c r="B8" s="51">
         <v>2</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="40"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="40"/>
-      <c r="N8" s="43"/>
+      <c r="E8" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" s="39"/>
+      <c r="L8" s="42"/>
+      <c r="M8" s="39"/>
+      <c r="N8" s="42"/>
     </row>
     <row r="9" spans="1:1029">
-      <c r="A9" s="28" t="s">
-        <v>69</v>
+      <c r="A9" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="55"/>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="39"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42" t="s">
+      <c r="E9" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="38"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="42" t="s">
+      <c r="I9" s="39"/>
+      <c r="J9" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="40"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="42"/>
-      <c r="N9" s="42"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
     </row>
     <row r="10" spans="1:1029">
-      <c r="A10" s="28" t="s">
-        <v>76</v>
+      <c r="A10" s="27" t="s">
+        <v>43</v>
       </c>
       <c r="B10" s="52"/>
       <c r="C10" s="55"/>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="K10" s="40"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
+      <c r="E10" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="39"/>
+      <c r="J10" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K10" s="39"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
     </row>
     <row r="11" spans="1:1029">
-      <c r="A11" s="28" t="s">
-        <v>77</v>
+      <c r="A11" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="55"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="39"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="40"/>
-      <c r="J11" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="K11" s="40"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="N11" s="42"/>
+      <c r="E11" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="39"/>
+      <c r="J11" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="39"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="N11" s="41"/>
     </row>
     <row r="12" spans="1:1029">
-      <c r="A12" s="28" t="s">
-        <v>78</v>
+      <c r="A12" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="55"/>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" s="39"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="40"/>
-      <c r="J12" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="K12" s="40"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
+      <c r="E12" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="38"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="I12" s="39"/>
+      <c r="J12" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
     </row>
     <row r="13" spans="1:1029">
-      <c r="A13" s="28" t="s">
-        <v>79</v>
+      <c r="A13" s="27" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="53"/>
       <c r="C13" s="56"/>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="39"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="40"/>
-      <c r="J13" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="K13" s="40"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-    </row>
-    <row r="14" spans="1:1029" ht="15.6">
-      <c r="A14" s="28" t="s">
-        <v>80</v>
+      <c r="E13" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="39"/>
+      <c r="J13" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" s="39"/>
+      <c r="L13" s="41"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+    </row>
+    <row r="14" spans="1:1029" ht="15.75">
+      <c r="A14" s="27" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>83</v>
+        <v>50</v>
       </c>
       <c r="D14" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:1029" ht="15.6">
-      <c r="A15" s="28" t="s">
-        <v>81</v>
+    <row r="15" spans="1:1029" ht="15.75">
+      <c r="A15" s="27" t="s">
+        <v>48</v>
       </c>
       <c r="B15" s="6">
         <v>4</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>84</v>
+        <v>51</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="16"/>
       <c r="H15" s="18"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:1029" ht="15.6">
-      <c r="A16" s="28" t="s">
-        <v>82</v>
+    <row r="16" spans="1:1029" ht="15.75">
+      <c r="A16" s="27" t="s">
+        <v>49</v>
       </c>
       <c r="B16" s="6">
         <v>5</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="D16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="22" t="s">
-        <v>52</v>
+      <c r="E16" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="16"/>
       <c r="H16" s="18"/>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:11" ht="72">
+      <c r="J16" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30">
       <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C17" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="60">
+      <c r="A18" s="6">
+        <v>16</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="8">
+        <v>200</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75">
+      <c r="A19" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="41"/>
+      <c r="J19" s="16"/>
+      <c r="L19" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75">
+      <c r="A20" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="6">
+        <v>2</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="41"/>
+      <c r="J20" s="16"/>
+      <c r="L20" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75">
+      <c r="A21" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="6">
+        <v>3</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="31"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="31"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="34"/>
+    </row>
+    <row r="22" spans="1:14" ht="30">
+      <c r="A22" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="8">
-        <v>200</v>
-      </c>
-      <c r="E17" s="21" t="s">
+      <c r="G22" s="33"/>
+      <c r="H22" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="31"/>
+      <c r="J22" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" s="31"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+      <c r="N22" s="33"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="6">
+        <v>5</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>91</v>
+      <c r="G23" s="33"/>
+      <c r="H23" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="31"/>
+      <c r="J23" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K23" s="31"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="33"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="6">
+        <v>6</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="30"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="31"/>
+      <c r="J24" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="31"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="33"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="6">
+        <v>7</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="30"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="31"/>
+      <c r="J25" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" s="31"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B26" s="6">
+        <v>8</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26" s="31"/>
+      <c r="J26" s="33" t="s">
+        <v>111</v>
+      </c>
+      <c r="K26" s="31"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+      <c r="N26" s="33"/>
+    </row>
+    <row r="27" spans="1:14" ht="45">
+      <c r="A27" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="6">
+        <v>9</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="21"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="41"/>
+      <c r="J27" s="16"/>
+      <c r="L27" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="45">
+      <c r="A28" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="41"/>
+      <c r="J28" s="16"/>
+      <c r="L28" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B2:B7"/>
+  <mergeCells count="3">
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="C8:C13"/>

</xml_diff>

<commit_message>
Manual Test Case Reporting
</commit_message>
<xml_diff>
--- a/ECS.xlsx
+++ b/ECS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Structures" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="119">
   <si>
     <t>Sr#</t>
   </si>
@@ -328,9 +328,6 @@
   </si>
   <si>
     <t>webvalidation_NFPromo_9270990234_Active_7_API_Passing</t>
-  </si>
-  <si>
-    <t>1(Start)(End)</t>
   </si>
   <si>
     <t>consume_data_2699.1mb</t>
@@ -572,7 +569,25 @@
     <t>10(End)</t>
   </si>
   <si>
+    <t>['ns3:MemberList']=find(['MSISDN']=639270990232;['TotalAllocated'])</t>
+  </si>
+  <si>
+    <t>1(Start)</t>
+  </si>
+  <si>
+    <t>(End)</t>
+  </si>
+  <si>
+    <t>ValidateStatusCode</t>
+  </si>
+  <si>
+    <t>ValidateResponseParams</t>
+  </si>
+  <si>
     <t>['ns3:MemberList']=find(['MSISDN']=639270s990232;['TotalAllocated'])</t>
+  </si>
+  <si>
+    <t>Main Test Step</t>
   </si>
 </sst>
 </file>
@@ -936,7 +951,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1071,6 +1086,9 @@
     <xf numFmtId="49" fontId="8" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="8" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1098,7 +1116,13 @@
     <xf numFmtId="49" fontId="8" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1567,16 +1591,16 @@
       <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" style="21" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="21" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="21" customWidth="1"/>
+    <col min="4" max="4" width="40.109375" style="21" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="21" customWidth="1"/>
     <col min="6" max="6" width="48" style="21" customWidth="1"/>
-    <col min="7" max="7" width="86.5703125" style="21" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="21"/>
+    <col min="7" max="7" width="86.5546875" style="21" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="25" customFormat="1" ht="45.75" customHeight="1">
@@ -1622,7 +1646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="409.5">
+    <row r="3" spans="1:7" ht="409.6">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -1642,7 +1666,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="47.25">
+    <row r="4" spans="1:7" ht="46.8">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1702,7 +1726,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="409.5">
+    <row r="7" spans="1:7" ht="409.6">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1719,10 +1743,10 @@
         <v>75</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="409.5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="409.6">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -1739,10 +1763,10 @@
         <v>75</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="409.5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="409.6">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1759,7 +1783,7 @@
         <v>75</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1798,35 +1822,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMO28"/>
+  <dimension ref="A1:AMP31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="36" style="6" customWidth="1"/>
-    <col min="7" max="7" width="13" style="6" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="22" style="6" customWidth="1"/>
-    <col min="10" max="10" width="55.7109375" style="6" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="21" style="6" customWidth="1"/>
-    <col min="15" max="1027" width="9.140625" style="12"/>
-    <col min="1028" max="1029" width="9.140625" style="13"/>
-    <col min="1030" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="9.109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="36.88671875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="8" customWidth="1"/>
+    <col min="5" max="6" width="27.44140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="36" style="6" customWidth="1"/>
+    <col min="8" max="8" width="13" style="6" customWidth="1"/>
+    <col min="9" max="9" width="30.5546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="22" style="6" customWidth="1"/>
+    <col min="11" max="11" width="55.6640625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="24.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="21" style="6" customWidth="1"/>
+    <col min="16" max="1028" width="9.109375" style="12"/>
+    <col min="1029" max="1030" width="9.109375" style="13"/>
+    <col min="1031" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1029" s="5" customFormat="1" ht="38.25">
+    <row r="1" spans="1:1030" s="5" customFormat="1" ht="41.4">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1842,34 +1866,36 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="10"/>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
       <c r="R1" s="10"/>
@@ -2882,17 +2908,18 @@
       <c r="AMK1" s="10"/>
       <c r="AML1" s="10"/>
       <c r="AMM1" s="10"/>
-      <c r="AMN1" s="11"/>
+      <c r="AMN1" s="10"/>
       <c r="AMO1" s="11"/>
-    </row>
-    <row r="2" spans="1:1029" ht="15.75">
+      <c r="AMP1" s="11"/>
+    </row>
+    <row r="2" spans="1:1030" ht="15.6">
       <c r="A2" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="49" t="s">
         <v>35</v>
       </c>
       <c r="D2" s="28" t="s">
@@ -2901,164 +2928,170 @@
       <c r="E2" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="30" t="s">
+      <c r="F2" s="29"/>
+      <c r="G2" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="31"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="34"/>
-    </row>
-    <row r="3" spans="1:1029" ht="30">
+      <c r="L2" s="31"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:1030" ht="28.8">
       <c r="A3" s="27" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="49"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33" t="s">
+      <c r="F3" s="35"/>
+      <c r="G3" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="31"/>
+      <c r="K3" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="31"/>
-      <c r="L3" s="33"/>
+      <c r="L3" s="31"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
-    </row>
-    <row r="4" spans="1:1029">
+      <c r="O3" s="33"/>
+    </row>
+    <row r="4" spans="1:1030">
       <c r="A4" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="45"/>
-      <c r="C4" s="49"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33" t="s">
+      <c r="F4" s="35"/>
+      <c r="G4" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="31"/>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="31"/>
+      <c r="K4" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="33"/>
+      <c r="L4" s="31"/>
       <c r="M4" s="33"/>
       <c r="N4" s="33"/>
-    </row>
-    <row r="5" spans="1:1029">
+      <c r="O4" s="33"/>
+    </row>
+    <row r="5" spans="1:1030">
       <c r="A5" s="27" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="45"/>
-      <c r="C5" s="49"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33" t="s">
+      <c r="F5" s="35"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="I5" s="31"/>
-      <c r="J5" s="33" t="s">
+      <c r="J5" s="31"/>
+      <c r="K5" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="33"/>
+      <c r="L5" s="31"/>
       <c r="M5" s="33"/>
       <c r="N5" s="33"/>
-    </row>
-    <row r="6" spans="1:1029">
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:1030">
       <c r="A6" s="27" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="45"/>
-      <c r="C6" s="49"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33" t="s">
+      <c r="F6" s="35"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="31"/>
-      <c r="J6" s="33" t="s">
+      <c r="J6" s="31"/>
+      <c r="K6" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="33"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="33"/>
       <c r="N6" s="33"/>
-    </row>
-    <row r="7" spans="1:1029">
+      <c r="O6" s="33"/>
+    </row>
+    <row r="7" spans="1:1030">
       <c r="A7" s="27" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="46"/>
-      <c r="C7" s="50"/>
+      <c r="C7" s="51"/>
       <c r="D7" s="28" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="31"/>
-      <c r="J7" s="33" t="s">
+      <c r="J7" s="31"/>
+      <c r="K7" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="33"/>
+      <c r="L7" s="31"/>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
-    </row>
-    <row r="8" spans="1:1029" ht="15.75">
+      <c r="O7" s="33"/>
+    </row>
+    <row r="8" spans="1:1030" ht="15.6">
       <c r="A8" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="51">
+      <c r="B8" s="52">
         <v>2</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="55" t="s">
         <v>42</v>
       </c>
       <c r="D8" s="36" t="s">
@@ -3067,151 +3100,157 @@
       <c r="E8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="42"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="42"/>
-    </row>
-    <row r="9" spans="1:1029">
+      <c r="L8" s="39"/>
+      <c r="M8" s="42"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="42"/>
+    </row>
+    <row r="9" spans="1:1030">
       <c r="A9" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="55"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="56"/>
       <c r="D9" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="38"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41" t="s">
+      <c r="F9" s="43"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="39"/>
-      <c r="J9" s="33" t="s">
+      <c r="J9" s="39"/>
+      <c r="K9" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="39"/>
-      <c r="L9" s="41"/>
+      <c r="L9" s="39"/>
       <c r="M9" s="41"/>
       <c r="N9" s="41"/>
-    </row>
-    <row r="10" spans="1:1029">
+      <c r="O9" s="41"/>
+    </row>
+    <row r="10" spans="1:1030">
       <c r="A10" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="52"/>
-      <c r="C10" s="55"/>
+      <c r="B10" s="53"/>
+      <c r="C10" s="56"/>
       <c r="D10" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41" t="s">
+      <c r="F10" s="43"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="39"/>
-      <c r="J10" s="33" t="s">
+      <c r="J10" s="39"/>
+      <c r="K10" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K10" s="39"/>
-      <c r="L10" s="41"/>
+      <c r="L10" s="39"/>
       <c r="M10" s="41"/>
       <c r="N10" s="41"/>
-    </row>
-    <row r="11" spans="1:1029">
+      <c r="O10" s="41"/>
+    </row>
+    <row r="11" spans="1:1030">
       <c r="A11" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="52"/>
-      <c r="C11" s="55"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="56"/>
       <c r="D11" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="38"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41" t="s">
+      <c r="F11" s="43"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="I11" s="39"/>
-      <c r="J11" s="33" t="s">
+      <c r="J11" s="39"/>
+      <c r="K11" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="K11" s="39"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41" t="s">
+      <c r="L11" s="39"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="41"/>
-    </row>
-    <row r="12" spans="1:1029">
+      <c r="O11" s="41"/>
+    </row>
+    <row r="12" spans="1:1030">
       <c r="A12" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="52"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="56"/>
       <c r="D12" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41" t="s">
+      <c r="F12" s="43"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="33" t="s">
+      <c r="J12" s="39"/>
+      <c r="K12" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="K12" s="39"/>
-      <c r="L12" s="41"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="41"/>
       <c r="N12" s="41"/>
-    </row>
-    <row r="13" spans="1:1029">
+      <c r="O12" s="41"/>
+    </row>
+    <row r="13" spans="1:1030">
       <c r="A13" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="56"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="36" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="38"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41" t="s">
+      <c r="F13" s="43"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="39"/>
-      <c r="J13" s="33" t="s">
+      <c r="J13" s="39"/>
+      <c r="K13" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="K13" s="39"/>
-      <c r="L13" s="41"/>
+      <c r="L13" s="39"/>
       <c r="M13" s="41"/>
       <c r="N13" s="41"/>
-    </row>
-    <row r="14" spans="1:1029" ht="15.75">
+      <c r="O13" s="41"/>
+    </row>
+    <row r="14" spans="1:1030" ht="15.6">
       <c r="A14" s="27" t="s">
         <v>47</v>
       </c>
@@ -3227,9 +3266,10 @@
       <c r="E14" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" spans="1:1029" ht="15.75">
+      <c r="F14" s="22"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="1:1030" ht="15.6">
       <c r="A15" s="27" t="s">
         <v>48</v>
       </c>
@@ -3245,12 +3285,13 @@
       <c r="E15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="18"/>
-      <c r="J15" s="16"/>
-    </row>
-    <row r="16" spans="1:1029" ht="15.75">
+      <c r="F15" s="22"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="18"/>
+      <c r="K15" s="16"/>
+    </row>
+    <row r="16" spans="1:1030" ht="15.6">
       <c r="A16" s="27" t="s">
         <v>49</v>
       </c>
@@ -3266,263 +3307,224 @@
       <c r="E16" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="18"/>
-      <c r="J16" s="16" t="s">
+      <c r="F16" s="21"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="18"/>
+      <c r="K16" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="L16" s="6" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="30">
+    <row r="17" spans="1:15" ht="15.6">
       <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="57" t="s">
+      <c r="D17" s="48" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J17" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="60">
+      <c r="F17" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:15" ht="28.8">
       <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="6">
+      <c r="C18" s="59"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="28.8">
+      <c r="B19" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C19" s="60"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="21"/>
+      <c r="K19" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="28.8">
+      <c r="A20" s="6">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6">
         <v>1</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C20" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D20" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="K20" s="9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="57.6">
+      <c r="A21" s="6">
+        <v>16</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="8">
         <v>200</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E21" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15.75">
-      <c r="A19" s="27" t="s">
+      <c r="F21" s="21"/>
+      <c r="K21" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.6">
+      <c r="A22" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B22" s="6">
         <v>1</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D19" s="57" t="s">
+      <c r="C22" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="21"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="41"/>
-      <c r="J19" s="16"/>
-      <c r="L19" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="15.75">
-      <c r="A20" s="27" t="s">
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="41"/>
+      <c r="K22" s="16"/>
+      <c r="M22" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15.6">
+      <c r="A23" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="6">
+        <v>2</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="41"/>
+      <c r="K23" s="16"/>
+      <c r="M23" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.6">
+      <c r="A24" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="6">
-        <v>2</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="21"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="41"/>
-      <c r="J20" s="16"/>
-      <c r="L20" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="15.75">
-      <c r="A21" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="6">
+      <c r="B24" s="6">
         <v>3</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="K21" s="31"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="31"/>
-      <c r="N21" s="34"/>
-    </row>
-    <row r="22" spans="1:14" ht="30">
-      <c r="A22" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="6">
-        <v>4</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="K22" s="31"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="27" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="6">
-        <v>5</v>
-      </c>
-      <c r="C23" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="I23" s="31"/>
-      <c r="J23" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="K23" s="31"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="B24" s="6">
-        <v>6</v>
-      </c>
       <c r="C24" s="47" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="30"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" s="31"/>
-      <c r="J24" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="K24" s="31"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-      <c r="N24" s="33"/>
-    </row>
-    <row r="25" spans="1:14">
+      <c r="E24" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="31"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="L24" s="31"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="31"/>
+      <c r="O24" s="34"/>
+    </row>
+    <row r="25" spans="1:15" ht="28.8">
       <c r="A25" s="27" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B25" s="6">
-        <v>7</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>108</v>
+        <v>4</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>105</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="E25" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="I25" s="31"/>
-      <c r="J25" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="K25" s="31"/>
-      <c r="L25" s="33"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="31"/>
+      <c r="K25" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" s="31"/>
       <c r="M25" s="33"/>
       <c r="N25" s="33"/>
-    </row>
-    <row r="26" spans="1:14">
+      <c r="O25" s="33"/>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="27" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B26" s="6">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26" s="47" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D26" s="28" t="s">
         <v>17</v>
@@ -3530,69 +3532,168 @@
       <c r="E26" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="30"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="31"/>
-      <c r="J26" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="K26" s="31"/>
-      <c r="L26" s="33"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="J26" s="31"/>
+      <c r="K26" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="31"/>
       <c r="M26" s="33"/>
       <c r="N26" s="33"/>
-    </row>
-    <row r="27" spans="1:14" ht="45">
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="6">
+        <v>6</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="35"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="J27" s="31"/>
+      <c r="K27" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="31"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="6">
+        <v>7</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="35"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="J28" s="31"/>
+      <c r="K28" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="31"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="6">
+        <v>8</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="35"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J29" s="31"/>
+      <c r="K29" s="33" t="s">
+        <v>110</v>
+      </c>
+      <c r="L29" s="31"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+    </row>
+    <row r="30" spans="1:15" ht="43.2">
+      <c r="A30" s="27" t="s">
+        <v>102</v>
+      </c>
+      <c r="B30" s="6">
+        <v>9</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="41"/>
+      <c r="K30" s="16"/>
+      <c r="M30" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="43.2">
+      <c r="A31" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="B27" s="6">
-        <v>9</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="15" t="s">
+      <c r="B31" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E27" s="21"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="41"/>
-      <c r="J27" s="16"/>
-      <c r="L27" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="45">
-      <c r="A28" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="21"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="41"/>
-      <c r="J28" s="16"/>
-      <c r="L28" s="9" t="s">
-        <v>98</v>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="41"/>
+      <c r="K31" s="16"/>
+      <c r="M31" s="9" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C2:C7"/>
     <mergeCell ref="B8:B13"/>
     <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C17:C19"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>